<commit_message>
Adding parameters from excel file part2
</commit_message>
<xml_diff>
--- a/User_Data.xlsx
+++ b/User_Data.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,6 +31,12 @@
       <sz val="11"/>
       <u val="single"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <color rgb="FF56A8F5"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,9 +60,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +410,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -486,6 +495,11 @@
           <t>Groguforever123</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Pass - That user exists</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -505,7 +519,7 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>mando200420252@gmail.com</t>
+          <t>mando200720252@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -516,6 +530,11 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>Groguforever123</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Pass - User Created</t>
         </is>
       </c>
     </row>
@@ -527,7 +546,7 @@
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>dldg20042025@gmail.com</t>
+          <t>dldg20072025@gmail.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -538,6 +557,11 @@
       <c r="F4" t="inlineStr">
         <is>
           <t>Groguforever123</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Pass - First  and last Name are not valid</t>
         </is>
       </c>
     </row>
@@ -554,7 +578,7 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>mando210420252@gmail.com</t>
+          <t>mando270420252@gmail.com</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -569,7 +593,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Failed - First isn't too long</t>
+          <t>Pass - First Name is not valid!</t>
         </is>
       </c>
     </row>
@@ -586,7 +610,7 @@
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>mando230420252@gmail.com</t>
+          <t>mando270420252@gmail.com</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -601,7 +625,116 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Failed - Lastname isn't too long</t>
+          <t>Pass - Last Name is not valid!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>test_negative_incorrect_format_email</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Pascal</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>dldg210461gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Groguforever123</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Groguforever123</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Pass - email is not valid!!</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>test_negative_password_Strength</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Grogu</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Pass - Not accurate Password!</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>test_positive_password_Strength</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Groguforever123</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Pass - Accurate Password!</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>test_negative_password_confirm_diff</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Pascal</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>mando20042028@gmail.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Groguforever123</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Groguforever123*</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Pass - Password and confirm are different</t>
         </is>
       </c>
     </row>
@@ -612,6 +745,8 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D4" r:id="rId3"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D5" r:id="rId4"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D7" display="dldg210461@gmail.com" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Adding documentation Test scripts
</commit_message>
<xml_diff>
--- a/User_Data.xlsx
+++ b/User_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="magento_new_users" sheetId="1" state="visible" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C20" sqref="C18:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -482,7 +482,7 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>mando20042028@gmail.com</t>
+          <t>mando24052025@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -519,7 +519,7 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>mando200720252@gmail.com</t>
+          <t>mando26052025@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Failed - It isn't possible to create a user</t>
+          <t>Pass - User Created</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pass - First  and last Name are not valid</t>
+          <t>Pass - First and last Name are not valid</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Modifying display in 1st screen,comments on conftest
</commit_message>
<xml_diff>
--- a/User_Data.xlsx
+++ b/User_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="magento_new_users" sheetId="1" state="visible" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C18:D20"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -472,27 +472,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pascal</t>
+          <t>Doe1</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>mando24052025@gmail.com</t>
+          <t>Forever24052025@gmail.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -509,27 +509,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pascal</t>
+          <t>Doe2</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>mando26052025@gmail.com</t>
+          <t>Forever26052025@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -551,12 +551,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -573,22 +573,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Pascal</t>
+          <t>Doe3</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>mando270420252@gmail.com</t>
+          <t>Forever270420252@gmail.com</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -605,22 +605,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>John</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>mando270420252@gmail.com</t>
+          <t>Forever270420252@gmail.com</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -637,12 +637,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Pascal</t>
+          <t>Doe4</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -652,12 +652,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -675,7 +675,7 @@
       <c r="D8" s="1" t="n"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Grogu</t>
+          <t>Forev</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -709,27 +709,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Pascal</t>
+          <t>Doe5</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>mando20042028@gmail.com</t>
+          <t>Forever20042028@gmail.com</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Groguforever123</t>
+          <t>Forever123</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Groguforever123*</t>
+          <t>Forever123*</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">

</xml_diff>